<commit_message>
Moved username/password to excel sheet
</commit_message>
<xml_diff>
--- a/Claimbot Template.xlsx
+++ b/Claimbot Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\ClaimBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE2CD9A-3E6A-4225-A2D2-E98841211ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1551C5BD-2BBA-40D3-ADA9-283156FD207A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -171,6 +171,18 @@
   </si>
   <si>
     <t>Auth End</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -273,15 +285,7 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
@@ -291,14 +295,24 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -588,259 +602,284 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7759B226-B548-469F-A5B2-76DE4BBA961D}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C7" sqref="C7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" style="11" customWidth="1"/>
-    <col min="2" max="3" width="8.7265625" style="11"/>
-    <col min="4" max="4" width="12.6328125" style="11" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="11"/>
+    <col min="1" max="1" width="12.6328125" style="10" customWidth="1"/>
+    <col min="2" max="3" width="8.7265625" style="10"/>
+    <col min="4" max="4" width="12.6328125" style="10" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="17"/>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-    </row>
-    <row r="7" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="12" t="s">
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="9" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="D7" s="12" t="s">
+      <c r="B9" s="15"/>
+      <c r="D9" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="19" t="s">
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="15" cm="1">
-        <f t="array" ref="B8">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A8 &amp; " 1")),Insurance_History!D:D,0),0))</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="13" t="s">
+      <c r="B10" s="13" cm="1">
+        <f t="array" ref="B10">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A10 &amp; " 1")),Insurance_History!D:D,0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="14"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="19" t="s">
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="15" cm="1">
-        <f t="array" ref="B9">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A9 &amp; " 1")),Insurance_History!D:D,0),0))</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="13" t="s">
+      <c r="B11" s="13" cm="1">
+        <f t="array" ref="B11">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A11 &amp; " 1")),Insurance_History!D:D,0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="14"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="15" cm="1">
-        <f t="array" ref="B10">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A10 &amp; " 1")),Insurance_History!D:D,0),0))</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="13" t="s">
+      <c r="B12" s="13" cm="1">
+        <f t="array" ref="B12">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A12 &amp; " 1")),Insurance_History!D:D,0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="15" cm="1">
-        <f t="array" ref="B11">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A11 &amp; " 1")),Insurance_History!D:D,0),0))</f>
+      <c r="B13" s="13" cm="1">
+        <f t="array" ref="B13">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A13 &amp; " 1")),Insurance_History!D:D,0),0))</f>
         <v>2</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="14"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="19" t="s">
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="15" cm="1">
-        <f t="array" ref="B12">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A12 &amp; " 1")),Insurance_History!D:D,0),0))</f>
+      <c r="B14" s="13" cm="1">
+        <f t="array" ref="B14">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A14 &amp; " 1")),Insurance_History!D:D,0),0))</f>
         <v>5</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D14" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="14"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="19" t="s">
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="15" cm="1">
-        <f t="array" ref="B13">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A13 &amp; " 1")),Insurance_History!D:D,0),0))</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="13" t="s">
+      <c r="B15" s="13" cm="1">
+        <f t="array" ref="B15">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A15 &amp; " 1")),Insurance_History!D:D,0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="14"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="19" t="s">
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="15" cm="1">
-        <f t="array" ref="B14">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A14 &amp; " 1")),Insurance_History!D:D,0),0))</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="13" t="s">
+      <c r="B16" s="13" cm="1">
+        <f t="array" ref="B16">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A16 &amp; " 1")),Insurance_History!D:D,0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="14"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="19" t="s">
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="15" cm="1">
-        <f t="array" ref="B15">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A15 &amp; " 1")),Insurance_History!D:D,0),0))</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="13" t="s">
+      <c r="B17" s="13" cm="1">
+        <f t="array" ref="B17">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A17 &amp; " 1")),Insurance_History!D:D,0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="14"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="19" t="s">
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="15" cm="1">
-        <f t="array" ref="B16">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A16 &amp; " 1")),Insurance_History!D:D,0),0))</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="13" t="s">
+      <c r="B18" s="13" cm="1">
+        <f t="array" ref="B18">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A18 &amp; " 1")),Insurance_History!D:D,0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="14"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="19" t="s">
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="15" cm="1">
-        <f t="array" ref="B17">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A17 &amp; " 1")),Insurance_History!D:D,0),0))</f>
-        <v>0</v>
-      </c>
-      <c r="D17" s="13" t="s">
+      <c r="B19" s="13" cm="1">
+        <f t="array" ref="B19">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A19 &amp; " 1")),Insurance_History!D:D,0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="14"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="19" t="s">
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="15" cm="1">
-        <f t="array" ref="B18">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A18 &amp; " 1")),Insurance_History!D:D,0),0))</f>
-        <v>0</v>
-      </c>
-      <c r="D18" s="13" t="s">
+      <c r="B20" s="13" cm="1">
+        <f t="array" ref="B20">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A20 &amp; " 1")),Insurance_History!D:D,0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="14"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="19" t="s">
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="15" cm="1">
-        <f t="array" ref="B19">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A19 &amp; " 1")),Insurance_History!D:D,0),0))</f>
-        <v>0</v>
-      </c>
-      <c r="D19" s="13" t="s">
+      <c r="B21" s="13" cm="1">
+        <f t="array" ref="B21">SUM(IF(ISNUMBER(Insurance_History!B:B),IF(MONTH(Insurance_History!B:B)=MONTH(DATEVALUE(A21 &amp; " 1")),Insurance_History!D:D,0),0))</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="14"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="19" t="s">
+      <c r="E21" s="12"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="15">
-        <f>SUM(B8:B19)</f>
+      <c r="B22" s="13">
+        <f>SUM(B10:B21)</f>
         <v>7</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D22" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="14">
-        <f>SUM(E8:E19)</f>
+      <c r="E22" s="12">
+        <f>SUM(E10:E21)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="L/8M3FcE705NU6neR17KLQIIMcykY96yen7iv2mRxLnyHpfJ8QwUFxSdAsq8RvalIdE1kuyfdOrJ2ej1b1EJbA==" saltValue="uED22h2jsnG353OJflURzA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="JxFbIcM+vpuOSyoUo+udb+kwc6MVYREhLTBr+zVB24/KAse0Rtnz4F6lqJbL+wC1z8atucrbGW4u77xxri+9dg==" saltValue="5OajXZajC7CChYk4KwHwjA==" spinCount="100000" sqref="A1:E1" name="Title"/>
   </protectedRanges>
-  <mergeCells count="9">
+  <mergeCells count="13">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D9:E9"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added notes to excel
</commit_message>
<xml_diff>
--- a/Claimbot Template.xlsx
+++ b/Claimbot Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\ClaimBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E57094D-430B-44BC-A967-6726C7B1C271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B8FA8C-EEB4-4733-AE2F-55C76F581914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -182,9 +182,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>Provider, Rending [123]</t>
-  </si>
-  <si>
     <t>Last Name</t>
   </si>
   <si>
@@ -204,6 +201,18 @@
   </si>
   <si>
     <t>Mary</t>
+  </si>
+  <si>
+    <t>Provider, Rendering [123]</t>
+  </si>
+  <si>
+    <t>facilities</t>
+  </si>
+  <si>
+    <t>Items must be written exactly the same</t>
+  </si>
+  <si>
+    <t>Payer and templates must match the tab name</t>
   </si>
 </sst>
 </file>
@@ -620,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7759B226-B548-469F-A5B2-76DE4BBA961D}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -634,7 +643,7 @@
     <col min="5" max="16384" width="8.7265625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="14" t="s">
         <v>29</v>
       </c>
@@ -643,7 +652,7 @@
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>11</v>
       </c>
@@ -653,30 +662,36 @@
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="16" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="16" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>36</v>
       </c>
@@ -687,7 +702,7 @@
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="18" t="s">
         <v>37</v>
       </c>
@@ -698,7 +713,7 @@
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="9" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="15" t="s">
         <v>14</v>
       </c>
@@ -708,7 +723,7 @@
       </c>
       <c r="E9" s="15"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -721,7 +736,7 @@
       </c>
       <c r="E10" s="12"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -734,7 +749,7 @@
       </c>
       <c r="E11" s="12"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -747,7 +762,7 @@
       </c>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -760,7 +775,7 @@
       </c>
       <c r="E13" s="12"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -773,7 +788,7 @@
       </c>
       <c r="E14" s="12"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -786,7 +801,7 @@
       </c>
       <c r="E15" s="12"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -910,7 +925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -927,13 +942,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -953,10 +968,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
         <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
       </c>
       <c r="C2" s="4">
         <v>20791</v>
@@ -979,10 +994,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
         <v>46</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
       </c>
       <c r="C3" s="4">
         <v>17699</v>

</xml_diff>

<commit_message>
Members loop for claims autofill
</commit_message>
<xml_diff>
--- a/Claimbot Template.xlsx
+++ b/Claimbot Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\ClaimBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B8FA8C-EEB4-4733-AE2F-55C76F581914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DA57C7-206B-40B3-9C3A-F2F2026BD06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -219,9 +219,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="167" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -304,7 +305,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -340,6 +341,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -631,7 +634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7759B226-B548-469F-A5B2-76DE4BBA961D}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -925,14 +928,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.1796875" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.26953125" bestFit="1" customWidth="1"/>
@@ -947,7 +951,7 @@
       <c r="B1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="19" t="s">
         <v>42</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -973,7 +977,7 @@
       <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="20">
         <v>20791</v>
       </c>
       <c r="D2" t="s">
@@ -999,7 +1003,7 @@
       <c r="B3" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="20">
         <v>17699</v>
       </c>
       <c r="D3" t="s">

</xml_diff>